<commit_message>
Update Project Plan ICSR, Theia.xlsx
</commit_message>
<xml_diff>
--- a/PSts/Project Plan ICSR, Theia.xlsx
+++ b/PSts/Project Plan ICSR, Theia.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27230"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{E6AD7CD5-F782-40E9-B28B-51FD83BC23EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A06EB5C7-BEB0-4C34-A828-69B2588524DC}"/>
+  <xr:revisionPtr revIDLastSave="333" documentId="8_{E6AD7CD5-F782-40E9-B28B-51FD83BC23EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3466E719-022C-4AC5-A39C-C2BA611EF185}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ICSR" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>Task</t>
   </si>
@@ -62,6 +62,9 @@
     <t>Prompt optimization</t>
   </si>
   <si>
+    <t>Nithin</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -71,112 +74,121 @@
     <t>Prompt examples</t>
   </si>
   <si>
+    <t>Not Started</t>
+  </si>
+  <si>
     <t>Output parsing to Json</t>
   </si>
   <si>
     <t>Developing API &amp; Testing</t>
   </si>
   <si>
+    <t>Sowmya Narayanan</t>
+  </si>
+  <si>
     <t>Integration with UI</t>
   </si>
   <si>
     <t>End to End Testing</t>
   </si>
   <si>
-    <t>Review</t>
+    <t>Entity Extraction From XML</t>
+  </si>
+  <si>
+    <t>Sowmya Narayanan / Pranathi</t>
+  </si>
+  <si>
+    <t>Yet to test - Format of the API response changed as per the UI requirment</t>
+  </si>
+  <si>
+    <t>Entity Extraction From Narrative</t>
+  </si>
+  <si>
+    <t>Narrative Generation</t>
+  </si>
+  <si>
+    <t>Yet to test - Format of the API response changed as per the Model requirment</t>
+  </si>
+  <si>
+    <t>Product Code</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Landing Page</t>
+  </si>
+  <si>
+    <t>UI development</t>
+  </si>
+  <si>
+    <t>Pranathi</t>
+  </si>
+  <si>
+    <t>New UI for ICSR</t>
+  </si>
+  <si>
+    <t>Reviewing the Figma wireframes</t>
   </si>
   <si>
     <t>Sai</t>
   </si>
   <si>
-    <t>Entity Extraction From XML</t>
-  </si>
-  <si>
-    <t>Sowmya Narayanan / Pranathi</t>
-  </si>
-  <si>
-    <t>Integrated testing in windows m/c needs to be done</t>
-  </si>
-  <si>
-    <t>Entity Extraction From Narrative</t>
-  </si>
-  <si>
-    <t>Narrative Generation</t>
-  </si>
-  <si>
-    <t>Product Code</t>
-  </si>
-  <si>
-    <t>Nithin / Pranathi</t>
-  </si>
-  <si>
-    <t>Landing Page</t>
-  </si>
-  <si>
-    <t>UI development</t>
-  </si>
-  <si>
-    <t>Pranathi</t>
-  </si>
-  <si>
-    <t>Integration of UI with backend</t>
+    <t>Deployment</t>
+  </si>
+  <si>
+    <t>Developing the app</t>
+  </si>
+  <si>
+    <t>Testing the app</t>
+  </si>
+  <si>
+    <t>Sai / Team</t>
+  </si>
+  <si>
+    <t>Mistral</t>
+  </si>
+  <si>
+    <t>Creating endpoint for mistral &amp; meditron</t>
   </si>
   <si>
     <t>Eswar</t>
   </si>
   <si>
-    <t>New UI for ICSR</t>
-  </si>
-  <si>
-    <t>Reviewing the Figma wireframes</t>
-  </si>
-  <si>
-    <t>Deployment</t>
-  </si>
-  <si>
-    <t>Building the docker image in dev</t>
+    <t>LLM Playground</t>
+  </si>
+  <si>
+    <t>Developing the UI</t>
+  </si>
+  <si>
+    <t>Sombir</t>
+  </si>
+  <si>
+    <t>Developing the backend code to inference the model with user input</t>
+  </si>
+  <si>
+    <t>API development</t>
+  </si>
+  <si>
+    <t>Yet to start</t>
+  </si>
+  <si>
+    <t>Eswar / Pranathi</t>
+  </si>
+  <si>
+    <t>End to End testing</t>
+  </si>
+  <si>
+    <t>Development</t>
   </si>
   <si>
     <t>Testing the app in dev</t>
   </si>
   <si>
-    <t>Sai / Team</t>
-  </si>
-  <si>
-    <t>Developing app in prod</t>
-  </si>
-  <si>
-    <t>Mistral</t>
-  </si>
-  <si>
-    <t>Creating endpoint for mistral &amp; meditron</t>
-  </si>
-  <si>
-    <t>LLM Playground</t>
-  </si>
-  <si>
-    <t>Developing the UI</t>
-  </si>
-  <si>
-    <t>Developing the backend code to inference the model with user input</t>
-  </si>
-  <si>
-    <t>API development</t>
-  </si>
-  <si>
-    <t>Eswar / Pranathi</t>
-  </si>
-  <si>
-    <t>End to End testing</t>
-  </si>
-  <si>
     <t>Doc QnA Chatbot</t>
   </si>
   <si>
     <t>Creating API for like, dislike</t>
-  </si>
-  <si>
-    <t>Nithin</t>
   </si>
   <si>
     <t>Creating API for comment</t>
@@ -433,9 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,20 +726,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="51.85546875" customWidth="1"/>
-    <col min="6" max="6" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -759,239 +769,293 @@
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45300</v>
+      </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45302</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45302</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>45302</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
       <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>18</v>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
       </c>
       <c r="F9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4"/>
+      <c r="D10" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="D12" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="4"/>
+      <c r="D13" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
       <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
         <v>16</v>
       </c>
+      <c r="C14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5">
+        <v>45300</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45302</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="B22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D20" s="5">
+        <v>45299</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C14:C15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -999,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFCC2C2C-2839-4A9D-8460-B58CDAF845D0}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="A5:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,6 +1075,8 @@
     <col min="2" max="2" width="40.140625" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1035,80 +1101,97 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>41</v>
+      </c>
+      <c r="D2" s="5">
+        <v>45301</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30.75">
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D3" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D4" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="D5" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D6" s="5">
+        <v>45301</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>31</v>
-      </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
-        <v>16</v>
+      <c r="E8" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1121,7 +1204,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C9" sqref="A9:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1154,102 +1237,102 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45.75">
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45.75">
       <c r="B6" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="45.75">
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30.75">
       <c r="B8" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30.75">
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30.75">
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30.75">
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30.75">
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1257,94 +1340,94 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1420,30 +1503,30 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="B3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="B5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1488,187 +1571,187 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="B4" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="B17" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="B18" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="B19" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="B21" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="B22" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="B23" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="B24" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="B25" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="B26" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="B27" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="B30" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>